<commit_message>
finished 2017 csv file
</commit_message>
<xml_diff>
--- a/data/2017.xlsx
+++ b/data/2017.xlsx
@@ -5,22 +5,22 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reva_\Dropbox\Rickettsiosis\Boletin de salud para datos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\reva_\Documents\GitHub\paper-rickettsiosis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7900" firstSheet="3" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7900" activeTab="10"/>
   </bookViews>
   <sheets>
-    <sheet name="sem01" sheetId="1" r:id="rId1"/>
-    <sheet name="sem02" sheetId="2" r:id="rId2"/>
-    <sheet name="sem03" sheetId="3" r:id="rId3"/>
-    <sheet name="sem04" sheetId="4" r:id="rId4"/>
-    <sheet name="sem05" sheetId="5" r:id="rId5"/>
-    <sheet name="sem06" sheetId="6" r:id="rId6"/>
-    <sheet name="sem07" sheetId="7" r:id="rId7"/>
-    <sheet name="sem08" sheetId="8" r:id="rId8"/>
-    <sheet name="sem09" sheetId="9" r:id="rId9"/>
+    <sheet name="sem1" sheetId="1" r:id="rId1"/>
+    <sheet name="sem2" sheetId="2" r:id="rId2"/>
+    <sheet name="sem3" sheetId="3" r:id="rId3"/>
+    <sheet name="sem4" sheetId="4" r:id="rId4"/>
+    <sheet name="sem5" sheetId="5" r:id="rId5"/>
+    <sheet name="sem6" sheetId="6" r:id="rId6"/>
+    <sheet name="sem7" sheetId="7" r:id="rId7"/>
+    <sheet name="sem8" sheetId="8" r:id="rId8"/>
+    <sheet name="sem9" sheetId="9" r:id="rId9"/>
     <sheet name="sem10" sheetId="10" r:id="rId10"/>
     <sheet name="sem11" sheetId="12" r:id="rId11"/>
     <sheet name="sem12" sheetId="11" r:id="rId12"/>

</xml_diff>